<commit_message>
latest to been added
</commit_message>
<xml_diff>
--- a/week03_report.xlsx
+++ b/week03_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t>Student ID</t>
   </si>
@@ -202,7 +202,7 @@
     <t>Week: Week03</t>
   </si>
   <si>
-    <t>Generated: 2023-09-13 04:31:48 PM</t>
+    <t>Generated: 2023-09-14 10:47:40 AM</t>
   </si>
 </sst>
 </file>
@@ -745,17 +745,14 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>